<commit_message>
BFI, MI, 241111 modified 3
</commit_message>
<xml_diff>
--- a/R/data/BFI241111.xlsx
+++ b/R/data/BFI241111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8737D4CA-A8D0-C146-813B-59352502B94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ED77D8-41BA-AE4A-9FB1-A1A5015DC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53980" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="295">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -906,6 +906,99 @@
   </si>
   <si>
     <t>윤병찬</t>
+  </si>
+  <si>
+    <t>minseok1937@gmail.com</t>
+  </si>
+  <si>
+    <t>경영</t>
+  </si>
+  <si>
+    <t>김민석</t>
+  </si>
+  <si>
+    <t>h20191240@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>홍이래</t>
+  </si>
+  <si>
+    <t>seollo020531@naver.com</t>
+  </si>
+  <si>
+    <t>소프트웨어학과</t>
+  </si>
+  <si>
+    <t>설창원</t>
+  </si>
+  <si>
+    <t>algus5661@naver.com</t>
+  </si>
+  <si>
+    <t>최미현</t>
+  </si>
+  <si>
+    <t>oepdwrtyy@gmail.com</t>
+  </si>
+  <si>
+    <t>강종현</t>
+  </si>
+  <si>
+    <t>eung4077@gmail.com</t>
+  </si>
+  <si>
+    <t>강은결</t>
+  </si>
+  <si>
+    <t>syw050819@naver.com</t>
+  </si>
+  <si>
+    <t>신예원</t>
+  </si>
+  <si>
+    <t>kimguswls6685@naver.com</t>
+  </si>
+  <si>
+    <t>콘텐츠IT전공</t>
+  </si>
+  <si>
+    <t>김현진</t>
+  </si>
+  <si>
+    <t>ertyhx3@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">광고홍보학과 </t>
+  </si>
+  <si>
+    <t>김미소</t>
+  </si>
+  <si>
+    <t>withhowon@gmail.com</t>
+  </si>
+  <si>
+    <t>서호원</t>
+  </si>
+  <si>
+    <t>snp040609@naver.com</t>
+  </si>
+  <si>
+    <t>박세나</t>
+  </si>
+  <si>
+    <t>mt1661@naver.com</t>
+  </si>
+  <si>
+    <t>콘탠츠IT전공</t>
+  </si>
+  <si>
+    <t>정성민</t>
+  </si>
+  <si>
+    <t>rer220@naver.com</t>
+  </si>
+  <si>
+    <t>김대명</t>
   </si>
 </sst>
 </file>
@@ -952,7 +1045,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1179,11 +1272,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1228,6 +1360,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1279,7 +1420,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AA96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AA109">
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -1514,11 +1655,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA96"/>
+  <dimension ref="A1:AA109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9504,6 +9645,1085 @@
         <v>34</v>
       </c>
     </row>
+    <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="7">
+        <v>45608.673058587963</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D97" s="8">
+        <v>20202915</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K97" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O97" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R97" s="8">
+        <v>3</v>
+      </c>
+      <c r="S97" s="8">
+        <v>3</v>
+      </c>
+      <c r="T97" s="8">
+        <v>10</v>
+      </c>
+      <c r="U97" s="8">
+        <v>4</v>
+      </c>
+      <c r="V97" s="8">
+        <v>3</v>
+      </c>
+      <c r="W97" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X97" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y97" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z97" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA97" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="4">
+        <v>45608.675921076385</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D98" s="5">
+        <v>20191240</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L98" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q98" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R98" s="5">
+        <v>5</v>
+      </c>
+      <c r="S98" s="5">
+        <v>6</v>
+      </c>
+      <c r="T98" s="5">
+        <v>9</v>
+      </c>
+      <c r="U98" s="5">
+        <v>14</v>
+      </c>
+      <c r="V98" s="5">
+        <v>7</v>
+      </c>
+      <c r="W98" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X98" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y98" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z98" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA98" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="7">
+        <v>45608.685173252314</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D99" s="8">
+        <v>20225175</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I99" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L99" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M99" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O99" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P99" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q99" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R99" s="8">
+        <v>4</v>
+      </c>
+      <c r="S99" s="8">
+        <v>5</v>
+      </c>
+      <c r="T99" s="8">
+        <v>8</v>
+      </c>
+      <c r="U99" s="8">
+        <v>12</v>
+      </c>
+      <c r="V99" s="8">
+        <v>8</v>
+      </c>
+      <c r="W99" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X99" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y99" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z99" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA99" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="4">
+        <v>45608.69253414352</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100" s="5">
+        <v>20242355</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K100" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O100" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P100" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R100" s="5">
+        <v>7</v>
+      </c>
+      <c r="S100" s="5">
+        <v>6</v>
+      </c>
+      <c r="T100" s="5">
+        <v>6</v>
+      </c>
+      <c r="U100" s="5">
+        <v>9</v>
+      </c>
+      <c r="V100" s="5">
+        <v>5</v>
+      </c>
+      <c r="W100" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X100" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y100" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z100" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA100" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="7">
+        <v>45608.69424950231</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D101" s="8">
+        <v>20241003</v>
+      </c>
+      <c r="E101" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H101" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q101" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R101" s="8">
+        <v>4</v>
+      </c>
+      <c r="S101" s="8">
+        <v>8</v>
+      </c>
+      <c r="T101" s="8">
+        <v>7</v>
+      </c>
+      <c r="U101" s="8">
+        <v>11</v>
+      </c>
+      <c r="V101" s="8">
+        <v>11</v>
+      </c>
+      <c r="W101" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X101" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y101" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z101" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA101" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="4">
+        <v>45608.765146342594</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D102" s="5">
+        <v>20242201</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N102" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R102" s="5">
+        <v>4</v>
+      </c>
+      <c r="S102" s="5">
+        <v>8</v>
+      </c>
+      <c r="T102" s="5">
+        <v>7</v>
+      </c>
+      <c r="U102" s="5">
+        <v>12</v>
+      </c>
+      <c r="V102" s="5">
+        <v>7</v>
+      </c>
+      <c r="W102" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X102" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y102" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z102" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA102" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="7">
+        <v>45608.831043483791</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D103" s="8">
+        <v>20246251</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="F103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J103" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K103" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L103" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P103" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q103" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R103" s="8">
+        <v>6</v>
+      </c>
+      <c r="S103" s="8">
+        <v>4</v>
+      </c>
+      <c r="T103" s="8">
+        <v>5</v>
+      </c>
+      <c r="U103" s="8">
+        <v>10</v>
+      </c>
+      <c r="V103" s="8">
+        <v>6</v>
+      </c>
+      <c r="W103" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X103" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y103" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z103" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA103" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="4">
+        <v>45608.83613487269</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D104" s="5">
+        <v>20215144</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R104" s="5">
+        <v>5</v>
+      </c>
+      <c r="S104" s="5">
+        <v>3</v>
+      </c>
+      <c r="T104" s="5">
+        <v>6</v>
+      </c>
+      <c r="U104" s="5">
+        <v>12</v>
+      </c>
+      <c r="V104" s="5">
+        <v>8</v>
+      </c>
+      <c r="W104" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X104" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y104" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z104" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA104" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="7">
+        <v>45608.846135671294</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D105" s="8">
+        <v>20242607</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K105" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L105" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N105" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P105" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q105" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R105" s="8">
+        <v>3</v>
+      </c>
+      <c r="S105" s="8">
+        <v>4</v>
+      </c>
+      <c r="T105" s="8">
+        <v>3</v>
+      </c>
+      <c r="U105" s="8">
+        <v>3</v>
+      </c>
+      <c r="V105" s="8">
+        <v>4</v>
+      </c>
+      <c r="W105" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X105" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y105" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z105" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA105" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="4">
+        <v>45608.849338796295</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D106" s="5">
+        <v>20246245</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N106" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P106" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q106" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R106" s="5">
+        <v>7</v>
+      </c>
+      <c r="S106" s="5">
+        <v>8</v>
+      </c>
+      <c r="T106" s="5">
+        <v>8</v>
+      </c>
+      <c r="U106" s="5">
+        <v>13</v>
+      </c>
+      <c r="V106" s="5">
+        <v>9</v>
+      </c>
+      <c r="W106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA106" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="7">
+        <v>45608.858754618057</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D107" s="8">
+        <v>20242957</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J107" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K107" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L107" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N107" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P107" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R107" s="8">
+        <v>9</v>
+      </c>
+      <c r="S107" s="8">
+        <v>7</v>
+      </c>
+      <c r="T107" s="8">
+        <v>6</v>
+      </c>
+      <c r="U107" s="8">
+        <v>10</v>
+      </c>
+      <c r="V107" s="8">
+        <v>6</v>
+      </c>
+      <c r="W107" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="X107" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y107" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z107" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA107" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="4">
+        <v>45608.861045162033</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D108" s="5">
+        <v>20215239</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J108" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K108" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L108" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M108" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O108" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P108" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R108" s="5">
+        <v>6</v>
+      </c>
+      <c r="S108" s="5">
+        <v>9</v>
+      </c>
+      <c r="T108" s="5">
+        <v>7</v>
+      </c>
+      <c r="U108" s="5">
+        <v>5</v>
+      </c>
+      <c r="V108" s="5">
+        <v>7</v>
+      </c>
+      <c r="W108" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X108" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y108" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z108" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA108" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="16">
+        <v>45608.862400868056</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D109" s="17">
+        <v>20205124</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="F109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G109" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I109" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q109" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="R109" s="17">
+        <v>2</v>
+      </c>
+      <c r="S109" s="17">
+        <v>5</v>
+      </c>
+      <c r="T109" s="17">
+        <v>5</v>
+      </c>
+      <c r="U109" s="17">
+        <v>7</v>
+      </c>
+      <c r="V109" s="17">
+        <v>5</v>
+      </c>
+      <c r="W109" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="X109" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y109" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z109" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA109" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BFI, MI, 241111 modified 5
</commit_message>
<xml_diff>
--- a/R/data/BFI241111.xlsx
+++ b/R/data/BFI241111.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3305A-215C-784D-B923-D25DF7B93D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4305C6-A7DD-F147-B484-E358E0300ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,12 +1103,950 @@
         </r>
       </text>
     </comment>
+    <comment ref="F199" authorId="0" shapeId="0" xr:uid="{4FBB1361-20F2-8C45-AAAB-2E9EC4B1D93A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G199" authorId="0" shapeId="0" xr:uid="{37B7DD48-A328-7C4A-8F09-F7D4CB8B3C07}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I199" authorId="0" shapeId="0" xr:uid="{5F74C69F-404D-BB4F-9599-97AA4FCBA37B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J199" authorId="0" shapeId="0" xr:uid="{44A0994B-CDEE-A142-B230-6EAD9A0D2290}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K199" authorId="0" shapeId="0" xr:uid="{7C411CDC-74D4-C14B-B41B-8E7060A03523}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L199" authorId="0" shapeId="0" xr:uid="{29B48AB3-F47F-F442-AAA5-0121375F2C71}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N199" authorId="0" shapeId="0" xr:uid="{520C38D9-4155-2F47-966C-6ECC25B9F7D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O199" authorId="0" shapeId="0" xr:uid="{723BA388-A688-184F-815B-FAF641E51194}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P199" authorId="0" shapeId="0" xr:uid="{67292260-F99A-214A-9F72-54FB49703FA4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q199" authorId="0" shapeId="0" xr:uid="{F4E0F1B2-3A8B-1147-9D84-68ED51CA719F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S199" authorId="0" shapeId="0" xr:uid="{9CDCC700-4882-2D40-9587-84B7A42B1589}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T199" authorId="0" shapeId="0" xr:uid="{EBD4D15D-3518-6044-B36E-4267DA7EB816}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U199" authorId="0" shapeId="0" xr:uid="{2DA48235-9D94-DF41-A72D-7B6E9555A1A6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V199" authorId="0" shapeId="0" xr:uid="{DB756329-C628-0243-85F8-F7ADADA3F661}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X199" authorId="0" shapeId="0" xr:uid="{A8DBADF1-3FA3-BC43-8BC4-5DA11ACFD297}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y199" authorId="0" shapeId="0" xr:uid="{93738AD1-5845-DB4C-A71D-A5B9A220AF12}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z199" authorId="0" shapeId="0" xr:uid="{226DFE2C-DB5F-5245-8A10-2FDC4FB5769E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F203" authorId="0" shapeId="0" xr:uid="{ABF2C0F8-62DA-5042-B4E5-D82DBEF8EB13}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H203" authorId="0" shapeId="0" xr:uid="{46F20216-4031-EB4D-A4E4-0DCB57BBB44B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J203" authorId="0" shapeId="0" xr:uid="{7DD6C9B2-1F27-7541-BAAF-7E8B448A5094}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K203" authorId="0" shapeId="0" xr:uid="{00C9AD67-C907-454E-8074-79461FBE8FBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M203" authorId="0" shapeId="0" xr:uid="{AA863A31-F105-1142-A11E-3130789A245D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N203" authorId="0" shapeId="0" xr:uid="{6B38E0D2-3808-9447-AF94-DF4457A6F246}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O203" authorId="0" shapeId="0" xr:uid="{BA1EEF7D-37B4-E943-A516-0108D82B3C20}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P203" authorId="0" shapeId="0" xr:uid="{D6F1BEDC-0ADE-3842-AA83-53093C7A5C38}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q203" authorId="0" shapeId="0" xr:uid="{4A5CFBC6-0D2A-A345-A2DF-7B990BDB2594}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R203" authorId="0" shapeId="0" xr:uid="{A974754A-ED8C-BE4F-95EB-8CE7D86A0868}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S203" authorId="0" shapeId="0" xr:uid="{22BB0667-7A73-DB4E-89F5-5632100C49F7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T203" authorId="0" shapeId="0" xr:uid="{A620E18F-80AC-8648-B39F-BC2CB8A1C757}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U203" authorId="0" shapeId="0" xr:uid="{69B8DB7A-693A-E34E-AEAA-5BF727F21502}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V203" authorId="0" shapeId="0" xr:uid="{809A2621-7745-904F-8BBD-A807BAB0A23F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W203" authorId="0" shapeId="0" xr:uid="{42C340F3-5C15-464A-9EF2-6F3A1C47626F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X203" authorId="0" shapeId="0" xr:uid="{318D0FDF-C828-2542-B48D-24C61927B6C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y203" authorId="0" shapeId="0" xr:uid="{175D7007-B5E9-0245-BE38-F464AA441348}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA203" authorId="0" shapeId="0" xr:uid="{C17C033E-2DF3-D24F-972F-C6F0547D4A5C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F205" authorId="0" shapeId="0" xr:uid="{96A2D2D1-285A-B540-BB2A-ED3EC37C8F4A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G205" authorId="0" shapeId="0" xr:uid="{6402860E-BA23-FC40-8CAF-D4451FB9428C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H205" authorId="0" shapeId="0" xr:uid="{BF8D6ADF-9C8F-3E4E-9BEB-031154C8732F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J205" authorId="0" shapeId="0" xr:uid="{1103850C-6060-FE44-8F71-965CA32B3EFE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L205" authorId="0" shapeId="0" xr:uid="{5DD4B6F7-2EC7-F44F-B3E3-8D6A429FD367}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M205" authorId="0" shapeId="0" xr:uid="{CB079A9D-B1B0-0C4E-86C4-75BCADA2D2AD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N205" authorId="0" shapeId="0" xr:uid="{87BE6C0A-535A-A344-96B6-3C2D176F7510}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O205" authorId="0" shapeId="0" xr:uid="{44D0EDEA-74E5-0B43-BA60-350CD262C2EC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P205" authorId="0" shapeId="0" xr:uid="{95609D40-E90A-B142-93F2-A247142B886C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q205" authorId="0" shapeId="0" xr:uid="{3EAA178B-929B-A646-B55A-3F25E8A4402A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R205" authorId="0" shapeId="0" xr:uid="{5ECB96EB-0C35-EE43-B332-8124F0524AD3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S205" authorId="0" shapeId="0" xr:uid="{4D357169-9BD2-814F-943A-E25B1DBDE224}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T205" authorId="0" shapeId="0" xr:uid="{C2599FB0-156C-FD43-B19F-47EC2E45E3D2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V205" authorId="0" shapeId="0" xr:uid="{A6CE7102-3701-A94D-96B0-EF4B9514C110}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W205" authorId="0" shapeId="0" xr:uid="{64ACFE54-9D3E-A841-8F7A-DC678E73E01C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y205" authorId="0" shapeId="0" xr:uid="{62A2BF42-A7E3-EE4E-8EC6-5FD911EB4A41}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z205" authorId="0" shapeId="0" xr:uid="{D4236515-FE9B-6542-9342-1A997A649E59}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA205" authorId="0" shapeId="0" xr:uid="{9EF48666-FEFF-404F-8EFD-215A922CDB2B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F215" authorId="0" shapeId="0" xr:uid="{ADA7FA00-C89E-0C4C-9E02-14F6FEF4BDD7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G215" authorId="0" shapeId="0" xr:uid="{94430787-51BB-4746-BD30-41A802A19113}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J215" authorId="0" shapeId="0" xr:uid="{363AED3A-1493-B444-8267-E1EDF0E2591F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M215" authorId="0" shapeId="0" xr:uid="{0E0795AD-C79A-CF45-A3E9-B9964D3FBAF1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O215" authorId="0" shapeId="0" xr:uid="{4831F4BF-346A-D84B-905D-CA31F493AAAC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P215" authorId="0" shapeId="0" xr:uid="{8C384C21-5773-A749-A361-17FCFFB2B777}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R215" authorId="0" shapeId="0" xr:uid="{A1318165-5F46-6F4D-A8CA-4211B3A9BC42}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S215" authorId="0" shapeId="0" xr:uid="{1FD65043-8DCD-154A-8C4A-74127E99C543}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T215" authorId="0" shapeId="0" xr:uid="{9B1FCBD2-640E-EE4F-B3CC-6D10BD541085}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U215" authorId="0" shapeId="0" xr:uid="{7A901686-6559-2544-8339-6C2E0E7468C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V215" authorId="0" shapeId="0" xr:uid="{A78FE727-7EE3-7E4A-8DC6-E77719D27C67}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X215" authorId="0" shapeId="0" xr:uid="{07734957-6C82-E34F-AA65-7ACEF54C5B2E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y215" authorId="0" shapeId="0" xr:uid="{B3A3CAFE-8A6C-214F-85A7-053640E9B5D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z215" authorId="0" shapeId="0" xr:uid="{43392FAF-95E9-D640-8BF0-BC2A198FE462}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>응답자가 이 값을 업데이트했습니다.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="533">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2512,6 +3450,201 @@
   </si>
   <si>
     <t>현민수</t>
+  </si>
+  <si>
+    <t>kmg0187@naver.com</t>
+  </si>
+  <si>
+    <t>김민지</t>
+  </si>
+  <si>
+    <t>uhan0802@gmail.com</t>
+  </si>
+  <si>
+    <t>디지털미디어콘텐츠</t>
+  </si>
+  <si>
+    <t>이유한</t>
+  </si>
+  <si>
+    <t>lg01022928122@gmail.com</t>
+  </si>
+  <si>
+    <t>권주용</t>
+  </si>
+  <si>
+    <t>ggamy3637@naver.com</t>
+  </si>
+  <si>
+    <t>러시아학과</t>
+  </si>
+  <si>
+    <t>최효윤</t>
+  </si>
+  <si>
+    <t>twenty__dec@naver.com</t>
+  </si>
+  <si>
+    <t>채희주</t>
+  </si>
+  <si>
+    <t>kcwel1109@gmail.com</t>
+  </si>
+  <si>
+    <t>고미연</t>
+  </si>
+  <si>
+    <t>tjwjddn1130@gmail.com</t>
+  </si>
+  <si>
+    <t>서정우</t>
+  </si>
+  <si>
+    <t>csm06125@naver.com</t>
+  </si>
+  <si>
+    <t>반도체디스플레이</t>
+  </si>
+  <si>
+    <t>박근태</t>
+  </si>
+  <si>
+    <t>yeel6945@naver.com</t>
+  </si>
+  <si>
+    <t>이수빈</t>
+  </si>
+  <si>
+    <t>ydchufd@naver.com</t>
+  </si>
+  <si>
+    <t>정유민</t>
+  </si>
+  <si>
+    <t>bvc023@naver.com</t>
+  </si>
+  <si>
+    <t>김수영</t>
+  </si>
+  <si>
+    <t>lion5166@naver.com</t>
+  </si>
+  <si>
+    <t>김정연</t>
+  </si>
+  <si>
+    <t>donghyun6652@gmail.com</t>
+  </si>
+  <si>
+    <t>한동현</t>
+  </si>
+  <si>
+    <t>ms071207@naver.com</t>
+  </si>
+  <si>
+    <t>바이오메디컬</t>
+  </si>
+  <si>
+    <t>gusquddus20@naver.com</t>
+  </si>
+  <si>
+    <t>현병연</t>
+  </si>
+  <si>
+    <t>jione0831@naver.com</t>
+  </si>
+  <si>
+    <t>윤지원</t>
+  </si>
+  <si>
+    <t>hanyeong09@naver.com</t>
+  </si>
+  <si>
+    <t>이한영</t>
+  </si>
+  <si>
+    <t>sinyewon12@gamail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">식품영양학과 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">신예원 </t>
+  </si>
+  <si>
+    <t>t01094887068@gmail.com</t>
+  </si>
+  <si>
+    <t>손민재</t>
+  </si>
+  <si>
+    <t>raon2812@naver.com</t>
+  </si>
+  <si>
+    <t>최라온</t>
+  </si>
+  <si>
+    <t>his86814189@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 융합과학수사학과</t>
+  </si>
+  <si>
+    <t>황인성</t>
+  </si>
+  <si>
+    <t>na1448@naver.com</t>
+  </si>
+  <si>
+    <t>강나현</t>
+  </si>
+  <si>
+    <t>123plokml123@gmail.com</t>
+  </si>
+  <si>
+    <t>지현배</t>
+  </si>
+  <si>
+    <t>houng5011@naver.com</t>
+  </si>
+  <si>
+    <t>홍성원</t>
+  </si>
+  <si>
+    <t>ginny1024@naver.com</t>
+  </si>
+  <si>
+    <t>김희원</t>
+  </si>
+  <si>
+    <t>riwon1226@gmail.com</t>
+  </si>
+  <si>
+    <t>김리원</t>
+  </si>
+  <si>
+    <t>asrud8755@naver.com</t>
+  </si>
+  <si>
+    <t>광고홍보학과</t>
+  </si>
+  <si>
+    <t>김민경</t>
+  </si>
+  <si>
+    <t>baeksa01@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>서휘도</t>
+  </si>
+  <si>
+    <t>smarthulk0318@naver.com</t>
+  </si>
+  <si>
+    <t>조성민</t>
+  </si>
+  <si>
+    <t>yumi0901gami@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2987,7 +4120,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AA190">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AA220">
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3222,11 +4355,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA190"/>
+  <dimension ref="A1:AA220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C196" sqref="C196"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C228" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19014,6 +20147,2496 @@
         <v>34</v>
       </c>
     </row>
+    <row r="191" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="7">
+        <v>45610.82606821759</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D191" s="8">
+        <v>20203802</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="F191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L191" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N191" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P191" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R191" s="8">
+        <v>6</v>
+      </c>
+      <c r="S191" s="8">
+        <v>6</v>
+      </c>
+      <c r="T191" s="8">
+        <v>8</v>
+      </c>
+      <c r="U191" s="8">
+        <v>8</v>
+      </c>
+      <c r="V191" s="8">
+        <v>8</v>
+      </c>
+      <c r="W191" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X191" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y191" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z191" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA191" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="192" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="4">
+        <v>45610.827074398148</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="D192" s="5">
+        <v>20212555</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G192" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J192" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M192" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N192" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O192" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q192" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R192" s="5">
+        <v>2</v>
+      </c>
+      <c r="S192" s="5">
+        <v>9</v>
+      </c>
+      <c r="T192" s="5">
+        <v>5</v>
+      </c>
+      <c r="U192" s="5">
+        <v>7</v>
+      </c>
+      <c r="V192" s="5">
+        <v>5</v>
+      </c>
+      <c r="W192" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X192" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y192" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z192" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA192" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="7">
+        <v>45610.837418842595</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D193" s="8">
+        <v>20215109</v>
+      </c>
+      <c r="E193" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H193" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I193" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J193" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L193" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N193" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O193" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q193" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R193" s="8">
+        <v>8</v>
+      </c>
+      <c r="S193" s="8">
+        <v>2</v>
+      </c>
+      <c r="T193" s="8">
+        <v>10</v>
+      </c>
+      <c r="U193" s="8">
+        <v>11</v>
+      </c>
+      <c r="V193" s="8">
+        <v>13</v>
+      </c>
+      <c r="W193" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X193" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y193" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z193" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA193" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="4">
+        <v>45610.857292858796</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="D194" s="5">
+        <v>20201733</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F194" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G194" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H194" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I194" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J194" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K194" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L194" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M194" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N194" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O194" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P194" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q194" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R194" s="5">
+        <v>3</v>
+      </c>
+      <c r="S194" s="5">
+        <v>10</v>
+      </c>
+      <c r="T194" s="5">
+        <v>8</v>
+      </c>
+      <c r="U194" s="5">
+        <v>9</v>
+      </c>
+      <c r="V194" s="5">
+        <v>12</v>
+      </c>
+      <c r="W194" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X194" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y194" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z194" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA194" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="195" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="7">
+        <v>45610.876661030095</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D195" s="8">
+        <v>20243959</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="F195" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G195" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I195" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J195" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K195" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L195" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M195" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N195" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O195" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P195" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q195" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R195" s="8">
+        <v>3</v>
+      </c>
+      <c r="S195" s="8">
+        <v>9</v>
+      </c>
+      <c r="T195" s="8">
+        <v>10</v>
+      </c>
+      <c r="U195" s="8">
+        <v>11</v>
+      </c>
+      <c r="V195" s="8">
+        <v>10</v>
+      </c>
+      <c r="W195" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X195" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y195" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z195" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA195" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="196" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="4">
+        <v>45610.881543379626</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D196" s="5">
+        <v>20246204</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="F196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H196" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L196" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N196" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O196" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P196" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q196" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R196" s="5">
+        <v>8</v>
+      </c>
+      <c r="S196" s="5">
+        <v>9</v>
+      </c>
+      <c r="T196" s="5">
+        <v>6</v>
+      </c>
+      <c r="U196" s="5">
+        <v>11</v>
+      </c>
+      <c r="V196" s="5">
+        <v>10</v>
+      </c>
+      <c r="W196" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X196" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y196" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z196" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA196" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="197" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="7">
+        <v>45610.921218240735</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D197" s="8">
+        <v>20213064</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="F197" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G197" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H197" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I197" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J197" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K197" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L197" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M197" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N197" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O197" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P197" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q197" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R197" s="8">
+        <v>6</v>
+      </c>
+      <c r="S197" s="8">
+        <v>8</v>
+      </c>
+      <c r="T197" s="8">
+        <v>6</v>
+      </c>
+      <c r="U197" s="8">
+        <v>11</v>
+      </c>
+      <c r="V197" s="8">
+        <v>4</v>
+      </c>
+      <c r="W197" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X197" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y197" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z197" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA197" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="198" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="4">
+        <v>45610.922839999999</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D198" s="5">
+        <v>20203321</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="F198" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H198" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K198" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L198" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O198" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P198" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R198" s="5">
+        <v>3</v>
+      </c>
+      <c r="S198" s="5">
+        <v>7</v>
+      </c>
+      <c r="T198" s="5">
+        <v>6</v>
+      </c>
+      <c r="U198" s="5">
+        <v>7</v>
+      </c>
+      <c r="V198" s="5">
+        <v>7</v>
+      </c>
+      <c r="W198" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X198" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y198" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z198" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA198" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="199" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="7">
+        <v>45610.959146099536</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D199" s="8">
+        <v>20203635</v>
+      </c>
+      <c r="E199" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="F199" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G199" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H199" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I199" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J199" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K199" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L199" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M199" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N199" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O199" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P199" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q199" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R199" s="8">
+        <v>6</v>
+      </c>
+      <c r="S199" s="8">
+        <v>10</v>
+      </c>
+      <c r="T199" s="8">
+        <v>9</v>
+      </c>
+      <c r="U199" s="8">
+        <v>9</v>
+      </c>
+      <c r="V199" s="8">
+        <v>10</v>
+      </c>
+      <c r="W199" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X199" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y199" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z199" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA199" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="200" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="4">
+        <v>45610.935316215277</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D200" s="5">
+        <v>20242363</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="F200" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G200" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H200" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I200" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J200" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K200" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L200" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M200" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N200" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O200" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P200" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q200" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R200" s="5">
+        <v>4</v>
+      </c>
+      <c r="S200" s="5">
+        <v>7</v>
+      </c>
+      <c r="T200" s="5">
+        <v>5</v>
+      </c>
+      <c r="U200" s="5">
+        <v>15</v>
+      </c>
+      <c r="V200" s="5">
+        <v>6</v>
+      </c>
+      <c r="W200" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X200" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y200" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z200" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA200" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="201" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A201" s="7">
+        <v>45610.936857280089</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C201" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D201" s="8">
+        <v>20217035</v>
+      </c>
+      <c r="E201" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="F201" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G201" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H201" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I201" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J201" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K201" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L201" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M201" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N201" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O201" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P201" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q201" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R201" s="8">
+        <v>4</v>
+      </c>
+      <c r="S201" s="8">
+        <v>7</v>
+      </c>
+      <c r="T201" s="8">
+        <v>10</v>
+      </c>
+      <c r="U201" s="8">
+        <v>5</v>
+      </c>
+      <c r="V201" s="8">
+        <v>8</v>
+      </c>
+      <c r="W201" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X201" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y201" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z201" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA201" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="202" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A202" s="4">
+        <v>45610.950900706019</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D202" s="5">
+        <v>20243612</v>
+      </c>
+      <c r="E202" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="F202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I202" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J202" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K202" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L202" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N202" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R202" s="5">
+        <v>8</v>
+      </c>
+      <c r="S202" s="5">
+        <v>8</v>
+      </c>
+      <c r="T202" s="5">
+        <v>8</v>
+      </c>
+      <c r="U202" s="5">
+        <v>9</v>
+      </c>
+      <c r="V202" s="5">
+        <v>9</v>
+      </c>
+      <c r="W202" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X202" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y202" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z202" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA202" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="203" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A203" s="7">
+        <v>45611.693238067128</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D203" s="8">
+        <v>20246300</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F203" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G203" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H203" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I203" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J203" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K203" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L203" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M203" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N203" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O203" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P203" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q203" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R203" s="8">
+        <v>6</v>
+      </c>
+      <c r="S203" s="8">
+        <v>3</v>
+      </c>
+      <c r="T203" s="8">
+        <v>5</v>
+      </c>
+      <c r="U203" s="8">
+        <v>12</v>
+      </c>
+      <c r="V203" s="8">
+        <v>9</v>
+      </c>
+      <c r="W203" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X203" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y203" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z203" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA203" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="204" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="4">
+        <v>45611.007350891203</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="D204" s="5">
+        <v>20193644</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G204" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J204" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K204" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O204" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P204" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q204" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R204" s="5">
+        <v>6</v>
+      </c>
+      <c r="S204" s="5">
+        <v>5</v>
+      </c>
+      <c r="T204" s="5">
+        <v>6</v>
+      </c>
+      <c r="U204" s="5">
+        <v>11</v>
+      </c>
+      <c r="V204" s="5">
+        <v>11</v>
+      </c>
+      <c r="W204" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X204" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y204" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z204" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA204" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="205" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="7">
+        <v>45611.399873935181</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D205" s="8">
+        <v>20227106</v>
+      </c>
+      <c r="E205" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="F205" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G205" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H205" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I205" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J205" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K205" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L205" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M205" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N205" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O205" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P205" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q205" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R205" s="8">
+        <v>8</v>
+      </c>
+      <c r="S205" s="8">
+        <v>6</v>
+      </c>
+      <c r="T205" s="8">
+        <v>8</v>
+      </c>
+      <c r="U205" s="8">
+        <v>9</v>
+      </c>
+      <c r="V205" s="8">
+        <v>10</v>
+      </c>
+      <c r="W205" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X205" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y205" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z205" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA205" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="206" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="4">
+        <v>45611.130040474542</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D206" s="5">
+        <v>20246262</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="F206" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H206" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K206" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L206" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M206" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O206" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P206" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R206" s="5">
+        <v>4</v>
+      </c>
+      <c r="S206" s="5">
+        <v>9</v>
+      </c>
+      <c r="T206" s="5">
+        <v>8</v>
+      </c>
+      <c r="U206" s="5">
+        <v>10</v>
+      </c>
+      <c r="V206" s="5">
+        <v>7</v>
+      </c>
+      <c r="W206" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X206" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y206" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z206" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA206" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="207" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="7">
+        <v>45611.408029837963</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="C207" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D207" s="8">
+        <v>20203423</v>
+      </c>
+      <c r="E207" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G207" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H207" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I207" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J207" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K207" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L207" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M207" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N207" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O207" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P207" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q207" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R207" s="8">
+        <v>4</v>
+      </c>
+      <c r="S207" s="8">
+        <v>7</v>
+      </c>
+      <c r="T207" s="8">
+        <v>8</v>
+      </c>
+      <c r="U207" s="8">
+        <v>13</v>
+      </c>
+      <c r="V207" s="8">
+        <v>9</v>
+      </c>
+      <c r="W207" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X207" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y207" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z207" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA207" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="208" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A208" s="4">
+        <v>45611.486042546298</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="D208" s="5">
+        <v>20243821</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R208" s="5">
+        <v>8</v>
+      </c>
+      <c r="S208" s="5">
+        <v>7</v>
+      </c>
+      <c r="T208" s="5">
+        <v>11</v>
+      </c>
+      <c r="U208" s="5">
+        <v>8</v>
+      </c>
+      <c r="V208" s="5">
+        <v>8</v>
+      </c>
+      <c r="W208" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X208" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y208" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z208" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA208" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="209" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="7">
+        <v>45611.565541585645</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D209" s="8">
+        <v>20242122</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="F209" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G209" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H209" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I209" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J209" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K209" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L209" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M209" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N209" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O209" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P209" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q209" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R209" s="8">
+        <v>2</v>
+      </c>
+      <c r="S209" s="8">
+        <v>3</v>
+      </c>
+      <c r="T209" s="8">
+        <v>3</v>
+      </c>
+      <c r="U209" s="8">
+        <v>3</v>
+      </c>
+      <c r="V209" s="8">
+        <v>2</v>
+      </c>
+      <c r="W209" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X209" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y209" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z209" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA209" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="210" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="4">
+        <v>45611.565922210648</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D210" s="5">
+        <v>20242751</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G210" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H210" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I210" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J210" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K210" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L210" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M210" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N210" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O210" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P210" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q210" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R210" s="5">
+        <v>8</v>
+      </c>
+      <c r="S210" s="5">
+        <v>5</v>
+      </c>
+      <c r="T210" s="5">
+        <v>8</v>
+      </c>
+      <c r="U210" s="5">
+        <v>12</v>
+      </c>
+      <c r="V210" s="5">
+        <v>8</v>
+      </c>
+      <c r="W210" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X210" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y210" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z210" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA210" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="211" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="7">
+        <v>45611.594175590275</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="C211" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="D211" s="8">
+        <v>20246942</v>
+      </c>
+      <c r="E211" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="F211" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G211" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H211" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I211" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J211" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K211" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L211" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M211" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N211" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O211" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P211" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q211" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R211" s="8">
+        <v>11</v>
+      </c>
+      <c r="S211" s="8">
+        <v>12</v>
+      </c>
+      <c r="T211" s="8">
+        <v>10</v>
+      </c>
+      <c r="U211" s="8">
+        <v>11</v>
+      </c>
+      <c r="V211" s="8">
+        <v>11</v>
+      </c>
+      <c r="W211" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X211" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y211" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z211" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA211" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="212" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A212" s="4">
+        <v>45611.595020474539</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D212" s="5">
+        <v>20243601</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H212" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I212" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L212" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N212" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P212" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q212" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R212" s="5">
+        <v>6</v>
+      </c>
+      <c r="S212" s="5">
+        <v>6</v>
+      </c>
+      <c r="T212" s="5">
+        <v>6</v>
+      </c>
+      <c r="U212" s="5">
+        <v>6</v>
+      </c>
+      <c r="V212" s="5">
+        <v>6</v>
+      </c>
+      <c r="W212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y212" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA212" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="213" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" s="7">
+        <v>45611.625830173609</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="C213" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D213" s="8">
+        <v>20245266</v>
+      </c>
+      <c r="E213" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="F213" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G213" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H213" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I213" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J213" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K213" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L213" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M213" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N213" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O213" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P213" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q213" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R213" s="8">
+        <v>7</v>
+      </c>
+      <c r="S213" s="8">
+        <v>5</v>
+      </c>
+      <c r="T213" s="8">
+        <v>4</v>
+      </c>
+      <c r="U213" s="8">
+        <v>8</v>
+      </c>
+      <c r="V213" s="8">
+        <v>4</v>
+      </c>
+      <c r="W213" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X213" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y213" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z213" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA213" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="214" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" s="4">
+        <v>45611.635482060185</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D214" s="5">
+        <v>20243741</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="F214" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G214" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H214" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I214" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J214" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K214" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L214" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M214" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N214" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O214" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P214" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q214" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R214" s="5">
+        <v>8</v>
+      </c>
+      <c r="S214" s="5">
+        <v>6</v>
+      </c>
+      <c r="T214" s="5">
+        <v>6</v>
+      </c>
+      <c r="U214" s="5">
+        <v>6</v>
+      </c>
+      <c r="V214" s="5">
+        <v>6</v>
+      </c>
+      <c r="W214" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X214" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y214" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z214" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA214" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="215" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="7">
+        <v>45611.682448159721</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="C215" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D215" s="8">
+        <v>20246233</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="F215" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G215" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J215" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M215" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O215" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P215" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q215" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R215" s="8">
+        <v>7</v>
+      </c>
+      <c r="S215" s="8">
+        <v>4</v>
+      </c>
+      <c r="T215" s="8">
+        <v>6</v>
+      </c>
+      <c r="U215" s="8">
+        <v>7</v>
+      </c>
+      <c r="V215" s="8">
+        <v>8</v>
+      </c>
+      <c r="W215" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="X215" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y215" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z215" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA215" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="216" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="4">
+        <v>45611.67044180556</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D216" s="5">
+        <v>20243704</v>
+      </c>
+      <c r="E216" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="F216" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G216" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H216" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I216" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J216" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K216" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L216" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M216" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N216" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O216" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P216" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q216" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R216" s="5">
+        <v>2</v>
+      </c>
+      <c r="S216" s="5">
+        <v>6</v>
+      </c>
+      <c r="T216" s="5">
+        <v>9</v>
+      </c>
+      <c r="U216" s="5">
+        <v>15</v>
+      </c>
+      <c r="V216" s="5">
+        <v>9</v>
+      </c>
+      <c r="W216" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X216" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y216" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z216" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA216" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="217" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A217" s="7">
+        <v>45611.676929687499</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="C217" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="D217" s="8">
+        <v>20222606</v>
+      </c>
+      <c r="E217" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="F217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H217" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J217" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L217" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N217" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O217" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P217" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q217" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R217" s="8">
+        <v>8</v>
+      </c>
+      <c r="S217" s="8">
+        <v>6</v>
+      </c>
+      <c r="T217" s="8">
+        <v>7</v>
+      </c>
+      <c r="U217" s="8">
+        <v>12</v>
+      </c>
+      <c r="V217" s="8">
+        <v>11</v>
+      </c>
+      <c r="W217" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="X217" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y217" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z217" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA217" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="218" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A218" s="4">
+        <v>45611.678064571759</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D218" s="5">
+        <v>20205188</v>
+      </c>
+      <c r="E218" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="F218" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G218" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H218" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I218" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J218" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K218" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L218" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M218" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N218" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O218" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P218" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q218" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R218" s="5">
+        <v>3</v>
+      </c>
+      <c r="S218" s="5">
+        <v>8</v>
+      </c>
+      <c r="T218" s="5">
+        <v>6</v>
+      </c>
+      <c r="U218" s="5">
+        <v>10</v>
+      </c>
+      <c r="V218" s="5">
+        <v>9</v>
+      </c>
+      <c r="W218" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X218" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y218" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z218" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA218" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="219" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A219" s="7">
+        <v>45611.683786354166</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="C219" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D219" s="8">
+        <v>20241095</v>
+      </c>
+      <c r="E219" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="F219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G219" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J219" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L219" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M219" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N219" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O219" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P219" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R219" s="8">
+        <v>6</v>
+      </c>
+      <c r="S219" s="8">
+        <v>8</v>
+      </c>
+      <c r="T219" s="8">
+        <v>7</v>
+      </c>
+      <c r="U219" s="8">
+        <v>11</v>
+      </c>
+      <c r="V219" s="8">
+        <v>9</v>
+      </c>
+      <c r="W219" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X219" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y219" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z219" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA219" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="220" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A220" s="13">
+        <v>45611.695487094912</v>
+      </c>
+      <c r="B220" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="C220" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D220" s="14">
+        <v>20241515</v>
+      </c>
+      <c r="E220" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="F220" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G220" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H220" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I220" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J220" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K220" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L220" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M220" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N220" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O220" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P220" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q220" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="R220" s="14">
+        <v>4</v>
+      </c>
+      <c r="S220" s="14">
+        <v>8</v>
+      </c>
+      <c r="T220" s="14">
+        <v>3</v>
+      </c>
+      <c r="U220" s="14">
+        <v>9</v>
+      </c>
+      <c r="V220" s="14">
+        <v>3</v>
+      </c>
+      <c r="W220" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="X220" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y220" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z220" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA220" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>